<commit_message>
Added poster and final BOM
</commit_message>
<xml_diff>
--- a/projectDocumentation/billOfMaterials.xlsx
+++ b/projectDocumentation/billOfMaterials.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mct81\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenAA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35DB1FD0-1660-46D5-847A-239F3241BE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F319A039-4B23-43A3-9FD2-AFC69BE6B542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1CDA5541-B098-BD48-88EB-683466DC232C}"/>
+    <workbookView xWindow="19090" yWindow="-3720" windowWidth="38620" windowHeight="21100" xr2:uid="{1CDA5541-B098-BD48-88EB-683466DC232C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="90">
   <si>
     <t>Name of Item</t>
   </si>
@@ -215,19 +213,124 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>IMC404</t>
+  </si>
+  <si>
+    <t>AFL-05</t>
+  </si>
+  <si>
+    <t>B08Q87MF19</t>
+  </si>
+  <si>
+    <t>Roboclaw 2x7A Motor Controller</t>
+  </si>
+  <si>
+    <t>Nibco 90 elbow pvc</t>
+  </si>
+  <si>
+    <t>Pololu</t>
+  </si>
+  <si>
+    <t>BASICMICRO</t>
+  </si>
+  <si>
+    <t>LampVPath</t>
+  </si>
+  <si>
+    <t>Loctite</t>
+  </si>
+  <si>
+    <t>Acejoz</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>NIBCO</t>
+  </si>
+  <si>
+    <t>Duracell</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Motor Controller</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Motor Bracket</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
+  </si>
+  <si>
+    <t>Super Glue</t>
+  </si>
+  <si>
+    <t>Fishing Line</t>
+  </si>
+  <si>
+    <t>PVC Pipe</t>
+  </si>
+  <si>
+    <t>PVC 90</t>
+  </si>
+  <si>
+    <t>AA Battery</t>
+  </si>
+  <si>
+    <t>12 V Metal Gear Motor</t>
+  </si>
+  <si>
+    <t>Pololu 25D mm Motor Bracket</t>
+  </si>
+  <si>
+    <t>AA Battery Holder with Lead Wires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear Fishing Wire, 656 ft </t>
+  </si>
+  <si>
+    <t>Loctite Super Glue Ultra Gel</t>
+  </si>
+  <si>
+    <t>20ft 2" schedule 40 pvc</t>
+  </si>
+  <si>
+    <t>28 Duracell AA batteries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0F1111"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -260,6 +363,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,20 +720,22 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.875" customWidth="1"/>
-    <col min="2" max="3" width="38.5" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="19.125" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="29.3984375" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.09765625" customWidth="1"/>
+    <col min="6" max="6" width="8.09765625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -670,7 +788,7 @@
         <v>22.68</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -697,7 +815,7 @@
         <v>8.41</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -724,7 +842,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -751,7 +869,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -778,7 +896,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -804,7 +922,7 @@
         <v>52.72</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -831,7 +949,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -858,7 +976,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -885,7 +1003,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -912,7 +1030,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -939,7 +1057,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -966,7 +1084,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -993,7 +1111,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1020,7 +1138,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1047,67 +1165,257 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4865</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>45.95</v>
+      </c>
       <c r="H17">
         <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>91.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2676</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>7.95</v>
+      </c>
+      <c r="H18">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>79.95</v>
+      </c>
+      <c r="H19">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>79.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="6">
+        <v>6543877239</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6.48</v>
+      </c>
+      <c r="H20">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1739050</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="H21">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <v>6.65</v>
+      </c>
+      <c r="H22">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="3">
+        <v>72000800</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>43.82</v>
+      </c>
+      <c r="H23">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>87.64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="7">
+        <v>39923215543</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4">
+        <v>5.15</v>
+      </c>
+      <c r="H24">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <v>14.69</v>
+      </c>
+      <c r="H25">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
+        <v>14.69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="5"/>
+      <c r="H26">
+        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="H18">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="H19">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="H20">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="H21">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="H22">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="H23">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="H24">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="H25">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="H26">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1116,19 +1424,19 @@
       </c>
       <c r="F27">
         <f>SUBTOTAL(109,Table2[Quantity])</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G27" t="s">
         <v>59</v>
       </c>
       <c r="H27">
         <f>SUBTOTAL(109,Table2[Total])</f>
-        <v>113.71</v>
+        <v>464.83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="90" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>